<commit_message>
Update Excel file with new content
</commit_message>
<xml_diff>
--- a/data/example_usage_profile_1.xlsx
+++ b/data/example_usage_profile_1.xlsx
@@ -236,7 +236,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,37 +249,37 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B7" s="1"/>
     </row>

</xml_diff>